<commit_message>
update menu laporan keuangan dan sms gateway
</commit_message>
<xml_diff>
--- a/data-siswa.xlsx
+++ b/data-siswa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>NIM</t>
   </si>
@@ -23,34 +23,25 @@
     <t>SISWA</t>
   </si>
   <si>
-    <t>T102137</t>
+    <t>081840</t>
+  </si>
+  <si>
+    <t>AYAH UJEB</t>
   </si>
   <si>
     <t>Rina</t>
   </si>
   <si>
-    <t>T102138</t>
-  </si>
-  <si>
-    <t>Khaira Bishry</t>
-  </si>
-  <si>
-    <t>T120139</t>
+    <t>Muhammad Khairu Mubarak Huzaifah</t>
+  </si>
+  <si>
+    <t>Abang Ujeb keren</t>
   </si>
   <si>
     <t>MUHAMMAD HUZAIFAH, S.Kom.</t>
   </si>
   <si>
-    <t>TIM102317</t>
-  </si>
-  <si>
-    <t>Abang Ujeb keren</t>
-  </si>
-  <si>
-    <t>TIM102318</t>
-  </si>
-  <si>
-    <t>Muhammad Khairu Mubarak Huzaifah</t>
+    <t>ira iru</t>
   </si>
 </sst>
 </file>
@@ -389,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -414,35 +405,43 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>24253</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>24524525</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3425115</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>64264647</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>67676647</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>